<commit_message>
Updated UT_RateCut.ipynb and calculations.xlsx
</commit_message>
<xml_diff>
--- a/data/calculations.xlsx
+++ b/data/calculations.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardevans/Docs/Economics/OSE/UT-RateCut/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA769436-12D2-6249-8BDC-8289BD7D99D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2613EE4-E1ED-9048-A21A-896F47DB72DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="19720" windowWidth="31900" windowHeight="14840" activeTab="1" xr2:uid="{DA92A03F-6D85-3D4B-A685-AC83812FC0E5}"/>
+    <workbookView xWindow="4760" yWindow="19720" windowWidth="31900" windowHeight="14840" xr2:uid="{DA92A03F-6D85-3D4B-A685-AC83812FC0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2" sheetId="6" r:id="rId1"/>
     <sheet name="Table 3" sheetId="2" r:id="rId2"/>
-    <sheet name="Cut 4.75" sheetId="1" r:id="rId3"/>
+    <sheet name="Cut 4.65" sheetId="1" r:id="rId3"/>
     <sheet name="Table 5" sheetId="5" r:id="rId4"/>
-    <sheet name="Table 7" sheetId="3" r:id="rId5"/>
-    <sheet name="Table 8 plus Baseline HH detail" sheetId="4" r:id="rId6"/>
+    <sheet name="Table 6" sheetId="3" r:id="rId5"/>
+    <sheet name="Table 7 plus Baseline HH detail" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,23 +41,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
   <si>
     <t>2023 General Session</t>
   </si>
   <si>
-    <t>H.B. 54</t>
-  </si>
-  <si>
-    <t>Rep. Steve Eliason, Sen. Daniel McCay</t>
-  </si>
-  <si>
-    <t>Corp rate cut</t>
-  </si>
-  <si>
-    <t>Pers rate cut</t>
-  </si>
-  <si>
     <t>FY2023</t>
   </si>
   <si>
@@ -76,9 +64,6 @@
     <t>Total revenues</t>
   </si>
   <si>
-    <t>4.85 to 4.8</t>
-  </si>
-  <si>
     <t>HB 240</t>
   </si>
   <si>
@@ -208,9 +193,6 @@
     <t>CIT pct IIT + CIT</t>
   </si>
   <si>
-    <t>Table 7</t>
-  </si>
-  <si>
     <t>Rate cut from 4.85%</t>
   </si>
   <si>
@@ -358,9 +340,6 @@
     <t>Reform</t>
   </si>
   <si>
-    <t>Rate cut to 4.75%</t>
-  </si>
-  <si>
     <t>High income household</t>
   </si>
   <si>
@@ -440,6 +419,12 @@
   </si>
   <si>
     <t>IIT rate</t>
+  </si>
+  <si>
+    <t>Table 6</t>
+  </si>
+  <si>
+    <t>Rate cut to 4.65%</t>
   </si>
 </sst>
 </file>
@@ -698,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -757,25 +742,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1091,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B2839-8054-B24E-81EE-2CBD0599259E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1102,106 +1084,107 @@
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>119</v>
       </c>
       <c r="B7" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8" s="5">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="40">
         <f>'Table 3'!B18/1000000</f>
         <v>51.684523069126755</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B9" s="5">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="40">
         <f>'Table 3'!D18/1000000</f>
         <v>143.84478734968673</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B10" s="5">
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="C10" s="42">
-        <f>'Cut 4.75'!R5/1000000</f>
-        <v>166.9888</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4.65E-2</v>
+      </c>
+      <c r="C10" s="40">
+        <f>'Cut 4.65'!L2/1000000</f>
+        <v>333.39017084149486</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B11" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C11" s="42">
-        <f>'Table 7'!H5/1000000</f>
-        <v>566.09203200000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="40">
+        <f>'Table 6'!H5/1000000</f>
+        <v>565.09633957633378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B12" s="5">
         <v>0.04</v>
       </c>
-      <c r="C12" s="42">
-        <f>'Table 7'!H6/1000000</f>
-        <v>1401.036032</v>
+      <c r="C12" s="40">
+        <f>'Table 6'!H6/1000000</f>
+        <v>1398.5717666800711</v>
       </c>
     </row>
   </sheetData>
@@ -1213,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0110904A-5926-7A48-881E-230978E1CFAF}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1225,60 +1208,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G1" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
+      <c r="G1" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="G2" s="44"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48" t="s">
-        <v>126</v>
+        <v>13</v>
+      </c>
+      <c r="G3" s="44"/>
+      <c r="J3" s="45" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48" t="s">
-        <v>127</v>
+      <c r="G4" s="44"/>
+      <c r="J4" s="45" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>3985.4</v>
@@ -1289,20 +1266,20 @@
       <c r="D5">
         <v>6771.9</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="48" t="s">
-        <v>128</v>
+      <c r="G5" s="44"/>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>355.9</v>
@@ -1313,25 +1290,25 @@
       <c r="D6">
         <v>937</v>
       </c>
-      <c r="G6" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="49">
+      <c r="G6" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="40">
         <f>C5</f>
         <v>6110.5</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="40">
         <f>D5</f>
         <v>6771.9</v>
       </c>
-      <c r="J6" s="50">
+      <c r="J6" s="46">
         <f>(I6-H6)/H6</f>
         <v>0.10823991490058091</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>10701.4</v>
@@ -1342,42 +1319,42 @@
       <c r="D7">
         <v>16020.1</v>
       </c>
-      <c r="G7" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="H7" s="49">
+      <c r="G7" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="40">
         <f>C7</f>
         <v>13965.6</v>
       </c>
-      <c r="I7" s="49">
+      <c r="I7" s="40">
         <f>D7</f>
         <v>16020.1</v>
       </c>
-      <c r="J7" s="50">
+      <c r="J7" s="46">
         <f>(I7-H7)/H7</f>
         <v>0.1471114739073151</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G8" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="51">
+      <c r="G8" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="2">
         <f>H6/H7</f>
         <v>0.43753938248267171</v>
       </c>
-      <c r="I8" s="51">
+      <c r="I8" s="2">
         <f>I6/I7</f>
         <v>0.42271271714908143</v>
       </c>
-      <c r="J8" s="50">
+      <c r="J8" s="46">
         <f>(I8-H8)/H8</f>
         <v>-3.388647040058726E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2">
         <f>B5/B7</f>
@@ -1391,22 +1368,22 @@
         <f>D5/D7</f>
         <v>0.42271271714908143</v>
       </c>
-      <c r="G9" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="H9" s="53">
+      <c r="G9" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="48">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="I9" s="53">
+      <c r="I9" s="48">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="49">
         <v>-1E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2">
         <f>B6/B7</f>
@@ -1423,7 +1400,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2">
         <f>B5/(B5+B6)</f>
@@ -1440,7 +1417,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2">
         <f>B6/(B5+B6)</f>
@@ -1462,41 +1439,41 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1">
         <v>56300000</v>
@@ -1508,7 +1485,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1">
         <f>B11*B17</f>
@@ -1534,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1673FC3-8F89-9346-AD20-607F921FFA03}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1554,265 +1531,214 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>96034000</v>
+        <v>379520000</v>
       </c>
       <c r="I2" s="1">
-        <v>96034000</v>
+        <v>379520000</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="L2" s="3">
-        <f>0.88*H2</f>
-        <v>84509920</v>
-      </c>
-      <c r="N2">
-        <v>0.05</v>
+        <f>'Table 3'!D11*H2</f>
+        <v>333390170.84149486</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>1669000</v>
+        <v>6670000</v>
       </c>
       <c r="H3" s="1">
-        <v>20182000</v>
+        <v>79630000</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="L3" s="3">
-        <f>0.12*H2</f>
-        <v>11524080</v>
+        <f>'Table 3'!D12*H2</f>
+        <v>46129829.158505104</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1">
         <f>SUM(G2:G3)</f>
-        <v>1669000</v>
+        <v>6670000</v>
       </c>
       <c r="H4" s="1">
-        <f>SUM(H2:H3)</f>
-        <v>116216000</v>
+        <f t="shared" ref="H4:I4" si="0">SUM(H2:H3)</f>
+        <v>459150000</v>
       </c>
       <c r="I4" s="1">
-        <f>SUM(I2:I3)</f>
-        <v>96034000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N5">
-        <v>0.1</v>
-      </c>
-      <c r="P5">
-        <f>N5/N2</f>
-        <v>2</v>
-      </c>
-      <c r="R5" s="3">
-        <f>L2*P6</f>
-        <v>166988800</v>
+        <f t="shared" si="0"/>
+        <v>379520000</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P6">
-        <f>P8/2</f>
-        <v>1.9759668450757024</v>
-      </c>
-      <c r="R6" s="3">
-        <f>0.5*L2+0.5*L7</f>
-        <v>209243760</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>379520000</v>
+        <v>734163000</v>
       </c>
       <c r="I7" s="1">
-        <v>379520000</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3">
-        <f>0.88*H7</f>
-        <v>333977600</v>
-      </c>
-      <c r="N7">
-        <v>0.2</v>
-      </c>
-      <c r="P7">
-        <f>N7/N2</f>
-        <v>4</v>
+        <v>734163000</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1">
-        <v>6670000</v>
+        <v>60488000</v>
       </c>
       <c r="H8" s="1">
-        <v>79630000</v>
+        <v>84061000</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="3">
-        <f>0.12*H7</f>
-        <v>45542400</v>
-      </c>
-      <c r="P8">
-        <f>L7/L2</f>
-        <v>3.9519336901514048</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
         <f>SUM(G7:G8)</f>
-        <v>6670000</v>
+        <v>60488000</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:I9" si="0">SUM(H7:H8)</f>
-        <v>459150000</v>
+        <f t="shared" ref="H9" si="1">SUM(H7:H8)</f>
+        <v>818224000</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="0"/>
-        <v>379520000</v>
+        <f t="shared" ref="I9" si="2">SUM(I7:I8)</f>
+        <v>734163000</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>734163000</v>
+        <v>192916000</v>
       </c>
       <c r="I12" s="1">
-        <v>734163000</v>
+        <v>192916000</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1">
-        <v>60488000</v>
+        <v>11455000</v>
       </c>
       <c r="H13" s="1">
-        <v>84061000</v>
+        <v>18010000</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1820,185 +1746,111 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G14" s="1">
         <f>SUM(G12:G13)</f>
-        <v>60488000</v>
+        <v>11455000</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14" si="1">SUM(H12:H13)</f>
-        <v>818224000</v>
+        <f t="shared" ref="H14" si="3">SUM(H12:H13)</f>
+        <v>210926000</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14" si="2">SUM(I12:I13)</f>
-        <v>734163000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+        <f t="shared" ref="I14" si="4">SUM(I12:I13)</f>
+        <v>192916000</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G19">
+        <v>6110.5</v>
+      </c>
+      <c r="H19">
+        <v>6771.9</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>742.7</v>
+      </c>
+      <c r="H20">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="G21">
+        <v>13965.6</v>
+      </c>
+      <c r="H21">
+        <v>16020.2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>192916000</v>
-      </c>
-      <c r="I17" s="1">
-        <v>192916000</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1">
-        <v>11455000</v>
-      </c>
-      <c r="H18" s="1">
-        <v>18010000</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1">
-        <f>SUM(G17:G18)</f>
-        <v>11455000</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" ref="H19" si="3">SUM(H17:H18)</f>
-        <v>210926000</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" ref="I19" si="4">SUM(I17:I18)</f>
-        <v>192916000</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="G23" t="s">
+      <c r="G23" s="2">
+        <f>G19/G21</f>
+        <v>0.43753938248267171</v>
+      </c>
+      <c r="H23" s="2">
+        <f>H19/H21</f>
+        <v>0.42271007852586107</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
         <v>25</v>
       </c>
-      <c r="H23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F24" t="s">
+      <c r="G24" s="2">
+        <f>G20/G21</f>
+        <v>5.3180672509595003E-2</v>
+      </c>
+      <c r="H24" s="2">
+        <f>H20/H21</f>
+        <v>5.8488658069187648E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="G24">
-        <v>6110.5</v>
-      </c>
-      <c r="H24">
-        <v>6771.9</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25">
-        <v>742.7</v>
-      </c>
-      <c r="H25">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G25" s="2">
+        <f>G19/(G19+G20)</f>
+        <v>0.89162726901301581</v>
+      </c>
+      <c r="H25" s="2">
+        <f>H19/(H19+H20)</f>
+        <v>0.87845217865065051</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
         <v>27</v>
       </c>
-      <c r="G26">
-        <v>13965.6</v>
-      </c>
-      <c r="H26">
-        <v>16020.2</v>
-      </c>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="2">
-        <f>G24/G26</f>
-        <v>0.43753938248267171</v>
-      </c>
-      <c r="H28" s="2">
-        <f>H24/H26</f>
-        <v>0.42271007852586107</v>
-      </c>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="2">
-        <f>G25/G26</f>
-        <v>5.3180672509595003E-2</v>
-      </c>
-      <c r="H29" s="2">
-        <f>H25/H26</f>
-        <v>5.8488658069187648E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="2">
-        <f>G24/(G24+G25)</f>
-        <v>0.89162726901301581</v>
-      </c>
-      <c r="H30" s="2">
-        <f>H24/(H24+H25)</f>
-        <v>0.87845217865065051</v>
-      </c>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="2">
-        <f>G25/(G24+G25)</f>
+      <c r="G26" s="2">
+        <f>G20/(G19+G20)</f>
         <v>0.10837273098698419</v>
       </c>
-      <c r="H31" s="2">
-        <f>H25/(H24+H25)</f>
+      <c r="H26" s="2">
+        <f>H20/(H19+H20)</f>
         <v>0.12154782134934945</v>
       </c>
     </row>
@@ -2012,7 +1864,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2022,100 +1874,100 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="41"/>
+      <c r="C3" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="51"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="B4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>98</v>
-      </c>
       <c r="H4" s="20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="H5" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -2125,7 +1977,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B8" s="34">
         <v>200000</v>
@@ -2134,26 +1986,28 @@
         <v>150505</v>
       </c>
       <c r="D8" s="35">
+        <f>B8-C8</f>
         <v>49495</v>
       </c>
       <c r="E8" s="34">
-        <v>150705</v>
+        <v>150905</v>
       </c>
       <c r="F8" s="35">
-        <v>49295</v>
+        <f>B8-E8</f>
+        <v>49095</v>
       </c>
       <c r="G8" s="1">
         <f>F8-D8</f>
-        <v>-200</v>
+        <v>-400</v>
       </c>
       <c r="H8" s="2">
         <f>G8/D8</f>
-        <v>-4.0408122032528542E-3</v>
+        <v>-8.0816244065057084E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B9" s="34">
         <v>80000</v>
@@ -2162,26 +2016,28 @@
         <v>69606</v>
       </c>
       <c r="D9" s="35">
+        <f>B9-C9</f>
         <v>10394</v>
       </c>
       <c r="E9" s="34">
-        <v>69686</v>
+        <v>69766</v>
       </c>
       <c r="F9" s="35">
-        <v>10314</v>
+        <f>B9-E9</f>
+        <v>10234</v>
       </c>
       <c r="G9" s="1">
         <f>F9-D9</f>
-        <v>-80</v>
+        <v>-160</v>
       </c>
       <c r="H9" s="2">
         <f>G9/D9</f>
-        <v>-7.696748123917645E-3</v>
+        <v>-1.539349624783529E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B10" s="34">
         <v>25000</v>
@@ -2190,12 +2046,14 @@
         <v>42138</v>
       </c>
       <c r="D10" s="35">
+        <f>B10-C10</f>
         <v>-17138</v>
       </c>
       <c r="E10" s="34">
         <v>42138</v>
       </c>
       <c r="F10" s="35">
+        <f>B10-E10</f>
         <v>-17138</v>
       </c>
       <c r="G10" s="1">
@@ -2209,7 +2067,7 @@
     </row>
     <row r="11" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
@@ -2221,7 +2079,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B12" s="34">
         <v>200000</v>
@@ -2230,12 +2088,14 @@
         <v>150505</v>
       </c>
       <c r="D12" s="35">
+        <f>B12-C12</f>
         <v>49495</v>
       </c>
       <c r="E12" s="34">
         <v>151161</v>
       </c>
       <c r="F12" s="35">
+        <f>B12-E12</f>
         <v>48839</v>
       </c>
       <c r="G12" s="1">
@@ -2249,7 +2109,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B13" s="34">
         <v>80000</v>
@@ -2258,12 +2118,14 @@
         <v>69606</v>
       </c>
       <c r="D13" s="35">
+        <f>B13-C13</f>
         <v>10394</v>
       </c>
       <c r="E13" s="34">
         <v>69886</v>
       </c>
       <c r="F13" s="35">
+        <f>B13-E13</f>
         <v>10114</v>
       </c>
       <c r="G13" s="1">
@@ -2277,7 +2139,7 @@
     </row>
     <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B14" s="38">
         <v>25000</v>
@@ -2286,12 +2148,14 @@
         <v>42138</v>
       </c>
       <c r="D14" s="39">
+        <f>B14-C14</f>
         <v>-17138</v>
       </c>
       <c r="E14" s="38">
         <v>42138</v>
       </c>
       <c r="F14" s="39">
+        <f>B14-E14</f>
         <v>-17138</v>
       </c>
       <c r="G14" s="12">
@@ -2305,7 +2169,7 @@
     </row>
     <row r="15" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -2317,7 +2181,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B16" s="34">
         <v>200000</v>
@@ -2326,12 +2190,14 @@
         <v>150505</v>
       </c>
       <c r="D16" s="35">
+        <f>B16-C16</f>
         <v>49495</v>
       </c>
       <c r="E16" s="34">
         <v>152161</v>
       </c>
       <c r="F16" s="35">
+        <f>B16-E16</f>
         <v>47839</v>
       </c>
       <c r="G16" s="1">
@@ -2345,7 +2211,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B17" s="34">
         <v>80000</v>
@@ -2354,12 +2220,14 @@
         <v>69606</v>
       </c>
       <c r="D17" s="35">
+        <f>B17-C17</f>
         <v>10394</v>
       </c>
       <c r="E17" s="34">
         <v>70286</v>
       </c>
       <c r="F17" s="35">
+        <f>B17-E17</f>
         <v>9714</v>
       </c>
       <c r="G17" s="1">
@@ -2373,7 +2241,7 @@
     </row>
     <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B18" s="38">
         <v>25000</v>
@@ -2382,12 +2250,14 @@
         <v>42138</v>
       </c>
       <c r="D18" s="39">
+        <f>B18-C18</f>
         <v>-17138</v>
       </c>
       <c r="E18" s="38">
         <v>42138</v>
       </c>
       <c r="F18" s="39">
+        <f>B18-E18</f>
         <v>-17138</v>
       </c>
       <c r="G18" s="12">
@@ -2414,7 +2284,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2424,56 +2294,57 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
         <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>4.7500000000000001E-2</v>
+        <v>4.65E-2</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>-80</v>
+        <v>-160</v>
       </c>
       <c r="E4" s="1">
-        <v>-200</v>
+        <v>-400</v>
       </c>
       <c r="H4" s="1">
-        <v>166988800</v>
+        <f>'Cut 4.65'!L2</f>
+        <v>333390170.84149486</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2490,30 +2361,30 @@
       </c>
       <c r="D5">
         <f>C5/C4</f>
-        <v>3.5</v>
+        <v>1.75</v>
       </c>
       <c r="E5" s="1">
         <v>-656</v>
       </c>
       <c r="F5">
         <f>E5/E4</f>
-        <v>3.28</v>
+        <v>1.64</v>
       </c>
       <c r="G5">
         <f>0.5*D5+0.5*F5</f>
-        <v>3.3899999999999997</v>
+        <v>1.6949999999999998</v>
       </c>
       <c r="H5" s="1">
         <f>G5*H4</f>
-        <v>566092032</v>
+        <v>565096339.57633376</v>
       </c>
       <c r="I5" s="1">
         <f>F5*H4</f>
-        <v>547723264</v>
+        <v>546759880.18005157</v>
       </c>
       <c r="J5" s="1">
         <f>D5*H4</f>
-        <v>584460800</v>
+        <v>583432798.97261596</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2528,30 +2399,30 @@
       </c>
       <c r="D6">
         <f>C6/C4</f>
-        <v>8.5</v>
+        <v>4.25</v>
       </c>
       <c r="E6" s="1">
         <v>-1656</v>
       </c>
       <c r="F6">
         <f>E6/E4</f>
-        <v>8.2799999999999994</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="G6">
         <f>0.5*D6+0.5*F6</f>
-        <v>8.39</v>
+        <v>4.1950000000000003</v>
       </c>
       <c r="H6" s="1">
         <f>G6*H4</f>
-        <v>1401036032</v>
+        <v>1398571766.6800711</v>
       </c>
       <c r="I6" s="1">
         <f>F6*H4</f>
-        <v>1382667264</v>
+        <v>1380235307.2837887</v>
       </c>
       <c r="J6" s="1">
         <f>D6*H4</f>
-        <v>1419404800</v>
+        <v>1416908226.0763531</v>
       </c>
     </row>
   </sheetData>
@@ -2576,39 +2447,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10">
@@ -2618,7 +2489,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
@@ -2629,7 +2500,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
@@ -2638,7 +2509,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
@@ -2647,7 +2518,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
@@ -2656,7 +2527,7 @@
     </row>
     <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -2665,7 +2536,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="18">
@@ -2676,7 +2547,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
@@ -2685,7 +2556,7 @@
     </row>
     <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
@@ -2694,7 +2565,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="18">
@@ -2705,7 +2576,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
@@ -2714,7 +2585,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
@@ -2723,7 +2594,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
@@ -2733,7 +2604,7 @@
     <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12">
@@ -2742,7 +2613,7 @@
     </row>
     <row r="19" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C19" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14">
@@ -2753,7 +2624,7 @@
     </row>
     <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16">
@@ -2770,34 +2641,34 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C25" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="10">
@@ -2807,7 +2678,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18">
@@ -2817,7 +2688,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
@@ -2826,7 +2697,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1">
@@ -2835,7 +2706,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
@@ -2844,7 +2715,7 @@
     </row>
     <row r="30" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1">
@@ -2853,7 +2724,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="18">
@@ -2863,7 +2734,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1">
@@ -2872,7 +2743,7 @@
     </row>
     <row r="33" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1">
@@ -2881,7 +2752,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C34" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="18">
@@ -2892,7 +2763,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1">
@@ -2901,7 +2772,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1">
@@ -2910,7 +2781,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1">
@@ -2920,7 +2791,7 @@
     <row r="38" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12">
@@ -2929,7 +2800,7 @@
     </row>
     <row r="39" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C39" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="14">
@@ -2940,7 +2811,7 @@
     </row>
     <row r="40" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16">
@@ -2952,34 +2823,34 @@
     <row r="41" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10">
@@ -2989,7 +2860,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C46" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18">
@@ -2999,7 +2870,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1">
@@ -3008,7 +2879,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1">
@@ -3017,7 +2888,7 @@
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1">
@@ -3026,7 +2897,7 @@
     </row>
     <row r="50" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1">
@@ -3035,7 +2906,7 @@
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C51" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="18">
@@ -3045,7 +2916,7 @@
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1">
@@ -3054,7 +2925,7 @@
     </row>
     <row r="53" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1">
@@ -3063,7 +2934,7 @@
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C54" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="18">
@@ -3074,7 +2945,7 @@
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1">
@@ -3083,7 +2954,7 @@
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1">
@@ -3092,7 +2963,7 @@
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1">
@@ -3102,7 +2973,7 @@
     <row r="58" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" s="12">
@@ -3111,7 +2982,7 @@
     </row>
     <row r="59" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C59" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="14">
@@ -3122,7 +2993,7 @@
     </row>
     <row r="60" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="16">

</xml_diff>